<commit_message>
add full backed in all page
</commit_message>
<xml_diff>
--- a/backend/formData.xlsx
+++ b/backend/formData.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -718,9 +718,92 @@
         <v>11/17/2024, 11:46:20 AM</v>
       </c>
     </row>
+    <row r="15">
+      <c r="B15" t="str">
+        <v>1-2 Weeks</v>
+      </c>
+      <c r="C15" t="str">
+        <v>tiwariravikant04@gmail.com</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Ravikant Tiwari</v>
+      </c>
+      <c r="E15" t="str">
+        <v>8744883594</v>
+      </c>
+      <c r="F15" t="str">
+        <v>+40</v>
+      </c>
+      <c r="G15" t="str">
+        <v>11/17/2024, 1:23:16 PM</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Life</v>
+      </c>
+      <c r="B16" t="str">
+        <v>1-2 Weeks</v>
+      </c>
+      <c r="C16" t="str">
+        <v>tiwariravikant04@gmail.com</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Ravikant Tiwari</v>
+      </c>
+      <c r="E16" t="str">
+        <v>8744883594</v>
+      </c>
+      <c r="F16" t="str">
+        <v>+40</v>
+      </c>
+      <c r="G16" t="str">
+        <v>11/17/2024, 1:40:24 PM</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="str">
+        <v>1week</v>
+      </c>
+      <c r="C17" t="str">
+        <v>tiwariravikant04@gmail.com</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Ravikant Tiwari</v>
+      </c>
+      <c r="E17" t="str">
+        <v>8744883594</v>
+      </c>
+      <c r="F17" t="str">
+        <v>+40</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Travel</v>
+      </c>
+      <c r="B18" t="str">
+        <v>1-2 Weeks</v>
+      </c>
+      <c r="C18" t="str">
+        <v>ravikanttiwari488@gmail.com</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Ravikant Tiwari</v>
+      </c>
+      <c r="E18" t="str">
+        <v>8744883594</v>
+      </c>
+      <c r="F18" t="str">
+        <v>+40</v>
+      </c>
+      <c r="G18" t="str">
+        <v>11/17/2024, 2:32:34 PM</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
all of setup done and also added all the secret to the ene file seperately and provided ene.example
</commit_message>
<xml_diff>
--- a/backend/formData.xlsx
+++ b/backend/formData.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -424,9 +424,6 @@
       <c r="G1" t="str">
         <v>readableTimestamp</v>
       </c>
-      <c r="H1" t="str">
-        <v>timestamp</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -801,9 +798,198 @@
         <v>11/17/2024, 2:32:34 PM</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Life</v>
+      </c>
+      <c r="B19" t="str">
+        <v>1-2 Weeks</v>
+      </c>
+      <c r="C19" t="str">
+        <v>ravikanttiwari488@gmail.com</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Ravikant Tiwari</v>
+      </c>
+      <c r="E19" t="str">
+        <v>8744883594</v>
+      </c>
+      <c r="F19" t="str">
+        <v>+40</v>
+      </c>
+      <c r="G19" t="str">
+        <v>11/17/2024, 11:51:39 PM</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Life</v>
+      </c>
+      <c r="B20" t="str">
+        <v>1-2 Weeks</v>
+      </c>
+      <c r="C20" t="str">
+        <v>ravikanttiwari488@gmail.com</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Ravikant Tiwari</v>
+      </c>
+      <c r="E20" t="str">
+        <v>8744883594</v>
+      </c>
+      <c r="F20" t="str">
+        <v>+40</v>
+      </c>
+      <c r="G20" t="str">
+        <v>11/17/2024, 11:57:02 PM</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Travel</v>
+      </c>
+      <c r="B21" t="str">
+        <v>1-2 Weeks</v>
+      </c>
+      <c r="C21" t="str">
+        <v>ravikanttiwari488@gmail.com</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Ravikant Tiwari</v>
+      </c>
+      <c r="E21" t="str">
+        <v>8744883594</v>
+      </c>
+      <c r="F21" t="str">
+        <v>+40</v>
+      </c>
+      <c r="G21" t="str">
+        <v>11/18/2024, 12:01:01 AM</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Life</v>
+      </c>
+      <c r="B22" t="str">
+        <v>1-2 Weeks</v>
+      </c>
+      <c r="C22" t="str">
+        <v>ravikanttiwari488@gmail.com</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Ravikant Tiwari</v>
+      </c>
+      <c r="E22" t="str">
+        <v>8744883594</v>
+      </c>
+      <c r="F22" t="str">
+        <v>+40</v>
+      </c>
+      <c r="G22" t="str">
+        <v>11/18/2024, 12:03:52 AM</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Life</v>
+      </c>
+      <c r="B23" t="str">
+        <v>1-2 Weeks</v>
+      </c>
+      <c r="C23" t="str">
+        <v>ravikanttiwari488@gmail.com</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Ravikant Tiwari</v>
+      </c>
+      <c r="E23" t="str">
+        <v>8744883594</v>
+      </c>
+      <c r="F23" t="str">
+        <v>+40</v>
+      </c>
+      <c r="G23" t="str">
+        <v>11/18/2024, 12:07:25 AM</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="str">
+        <v>1week</v>
+      </c>
+      <c r="C24" t="str">
+        <v>ravikanttiwari488@gmail.com</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Ravikant Tiwari</v>
+      </c>
+      <c r="E24" t="str">
+        <v>8744883594</v>
+      </c>
+      <c r="F24" t="str">
+        <v>+40</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Life</v>
+      </c>
+      <c r="B25" t="str">
+        <v>1-2 Weeks</v>
+      </c>
+      <c r="C25" t="str">
+        <v>ravikanttiwari488@gmail.com</v>
+      </c>
+      <c r="D25" t="str">
+        <v>Ravikant Tiwari</v>
+      </c>
+      <c r="E25" t="str">
+        <v>8744883594</v>
+      </c>
+      <c r="F25" t="str">
+        <v>+40</v>
+      </c>
+      <c r="G25" t="str">
+        <v>11/18/2024, 12:27:26 AM</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="str">
+        <v>1week</v>
+      </c>
+      <c r="C26" t="str">
+        <v>rktindia2003@gmail.com</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Ruchika kumari</v>
+      </c>
+      <c r="E26" t="str">
+        <v>9650511578</v>
+      </c>
+      <c r="F26" t="str">
+        <v>+40</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="str">
+        <v>2week</v>
+      </c>
+      <c r="C27" t="str">
+        <v>ravikanttiwari488@gmail.com</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Ravikant Tiwari</v>
+      </c>
+      <c r="E27" t="str">
+        <v>8744883594</v>
+      </c>
+      <c r="F27" t="str">
+        <v>+40</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G27"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>